<commit_message>
testei o contador de cadastro
</commit_message>
<xml_diff>
--- a/MotoristasRegistro.xlsx
+++ b/MotoristasRegistro.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -662,15 +662,11 @@
           <t>Rafael evander carvalho</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>33225726842</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>11995037548</t>
-        </is>
+      <c r="B6" t="n">
+        <v>33225726842</v>
+      </c>
+      <c r="C6" t="n">
+        <v>11995037548</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -693,6 +689,124 @@
         </is>
       </c>
       <c r="I6" t="inlineStr">
+        <is>
+          <t>Completo</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Renan rosa</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>48267379800</v>
+      </c>
+      <c r="C7" t="n">
+        <v>11978813206</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Atibaia-SP</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>TAC</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>23/04/2025 13:56</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Completo</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Fabiano felski</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1238946976</v>
+      </c>
+      <c r="C8" t="n">
+        <v>49991863317</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>são miguel do oeste-sc</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>TAC</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>23/04/2025 14:13</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Completo</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Gustavo Tedesco Bedin</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10854057960</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>49991878706</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>São Miguel Do Oeste-SC</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>TAC</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>23/04/2025 15:11</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>Completo</t>
         </is>
@@ -728,7 +842,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -867,15 +981,11 @@
           <t>JOSELMA GASPAR GREGORIO</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>35263195885</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>19994564565</t>
-        </is>
+      <c r="B4" t="n">
+        <v>35263195885</v>
+      </c>
+      <c r="C4" t="n">
+        <v>19994564565</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -899,6 +1009,88 @@
         </is>
       </c>
       <c r="I4" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Thaina Cristina Ramos de Oliveira</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>45693627888</v>
+      </c>
+      <c r="C5" t="n">
+        <v>19995305329</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Mogi Mirim-SP</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>AGREGADO</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>FTW-7533</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>23/04/2025 14:48</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Em andamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Rodrigo Rocha de Castro</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10003477967</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>49988681357</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Caçador-sc</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>AGREGADO</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>QJI-9564</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>23/04/2025 15:17</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>Em andamento</t>
         </is>

</xml_diff>